<commit_message>
Updates to a few files in downloads
</commit_message>
<xml_diff>
--- a/bin-release/files/Data_archive_pesticide.xlsx
+++ b/bin-release/files/Data_archive_pesticide.xlsx
@@ -1,31 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Atlantic_Aquifers\Data\Trends_data_analysis\Cycle 1_2\Web_Mapper_Files\for_review\4_Post_Editorial\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="19200" windowHeight="11520" tabRatio="823"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="19200" windowHeight="11520" tabRatio="823" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="2" r:id="rId1"/>
-    <sheet name="Pesticide_data" sheetId="3" r:id="rId2"/>
+    <sheet name="Statistical Results" sheetId="4" r:id="rId2"/>
+    <sheet name="Pesticide_data" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Pesticide_data!$A$1:$P$1</definedName>
-    <definedName name="WQdata_pest_final_Crosstab_remark" localSheetId="1">Pesticide_data!$B$1:$I$2543</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Pesticide_data!$A$1:$P$1</definedName>
+    <definedName name="WQdata_pest_final_Crosstab_remark" localSheetId="2">Pesticide_data!$B$1:$I$2543</definedName>
     <definedName name="WQdata_pest_final_Crosstab_remark">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2600" uniqueCount="1371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3166" uniqueCount="1396">
   <si>
     <t>261656081245901</t>
   </si>
@@ -4185,14 +4181,91 @@
   <si>
     <t>Total of 2,542 samples (1,271 pairs). Data for 6 pesticides after pesticide recovery corrections and after &lt; values were replaced with values slightly below the minimum detected concentration. These data were used to complete the Wilcoxon Pratt signed rank test using the low reporting level approach.</t>
   </si>
+  <si>
+    <t>Data included</t>
+  </si>
+  <si>
+    <t>Statistical results</t>
+  </si>
+  <si>
+    <t>Results of statistical analysis using Wilcoxon-Pratt signed rank test. For each constituent and each network, the probability value is given (p value), the number of samples available for analysis (N), and the median of the differences between the first and second sample (Median difference). If the statistical result was no significant change (p value greater than 0.10) no median difference is given (N/A). If a network has no samples, or fewer than 10 pairs of samples, that network is designated as having 'Insufficient data'</t>
+  </si>
+  <si>
+    <t>Dieldrin</t>
+  </si>
+  <si>
+    <t>Atrazine</t>
+  </si>
+  <si>
+    <t>Deethylatrazine</t>
+  </si>
+  <si>
+    <t>Simazine</t>
+  </si>
+  <si>
+    <t>Metolachlor</t>
+  </si>
+  <si>
+    <t>Prometon</t>
+  </si>
+  <si>
+    <t>p value</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Median Difference</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>acadsus1</t>
+  </si>
+  <si>
+    <t>Insufficient Data</t>
+  </si>
+  <si>
+    <t>delrsus1</t>
+  </si>
+  <si>
+    <t>dlmvluscr1</t>
+  </si>
+  <si>
+    <t>dlmvsus1</t>
+  </si>
+  <si>
+    <t>grsllusrc1</t>
+  </si>
+  <si>
+    <t>ltenlusag1</t>
+  </si>
+  <si>
+    <t>mobllusrc1</t>
+  </si>
+  <si>
+    <t>rioglusrc1</t>
+  </si>
+  <si>
+    <t>&lt;0.001</t>
+  </si>
+  <si>
+    <t>sofllusrc1a</t>
+  </si>
+  <si>
+    <t>uirbluscr1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.????"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="26" x14ac:knownFonts="1">
     <font>
@@ -4379,7 +4452,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4559,8 +4632,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -4672,6 +4751,26 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4838,7 +4937,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4865,9 +4964,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4887,6 +4983,70 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="106" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="33" borderId="0" xfId="106" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" xfId="106" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="106" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="33" borderId="0" xfId="106" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="106" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="7" fillId="33" borderId="0" xfId="106" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="7" fillId="0" borderId="0" xfId="106" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5114,7 +5274,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5149,7 +5309,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5358,10 +5518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5379,246 +5539,264 @@
       </c>
     </row>
     <row r="2" spans="1:4" s="7" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="21" t="s">
         <v>1353</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
         <v>1216</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="22" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="25" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>1373</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>1217</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+    <row r="6" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
         <v>1334</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>1370</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+    <row r="8" spans="1:4" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
         <v>1355</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B8" s="17" t="s">
         <v>1347</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C8" s="18" t="s">
         <v>1351</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D8" s="18" t="s">
         <v>1352</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+    <row r="9" spans="1:4" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>1348</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>1357</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+    <row r="10" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
         <v>1346</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>1356</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+    <row r="11" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>1218</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>1349</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+    <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
         <v>1220</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B12" s="10" t="s">
         <v>1358</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C12" s="20">
         <v>1E-3</v>
       </c>
-      <c r="D10" s="21">
-        <v>9.8999999999999999E-4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
+      <c r="D12" s="20">
+        <v>9.8999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
         <v>1335</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B13" s="10" t="s">
         <v>1359</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C13" s="20">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="D11" s="21">
-        <v>1.2899999999999999E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
+      <c r="D13" s="20">
+        <v>1.2899999999999999E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
         <v>1336</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B14" s="10" t="s">
         <v>1360</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C14" s="20">
         <v>1.952E-3</v>
       </c>
-      <c r="D12" s="21">
-        <v>1.951E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+      <c r="D14" s="20">
+        <v>1.951E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
         <v>1337</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B15" s="10" t="s">
         <v>1361</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C15" s="20">
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="D13" s="21">
-        <v>1.6900000000000001E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="D15" s="20">
+        <v>1.6900000000000001E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
         <v>1338</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B16" s="10" t="s">
         <v>1362</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C16" s="20">
         <v>1.66E-4</v>
       </c>
-      <c r="D14" s="21">
-        <v>1.65E-4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
+      <c r="D16" s="20">
+        <v>1.65E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
         <v>1339</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B17" s="10" t="s">
         <v>1363</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C17" s="20">
         <v>1E-3</v>
       </c>
-      <c r="D15" s="21">
-        <v>9.8999999999999999E-4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="D17" s="20">
+        <v>9.8999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
         <v>1219</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B18" s="11" t="s">
         <v>1350</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-    </row>
-    <row r="17" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+    </row>
+    <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
         <v>1340</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B19" s="10" t="s">
         <v>1364</v>
       </c>
-      <c r="C17" s="21">
+      <c r="C19" s="20">
         <v>1E-3</v>
       </c>
-      <c r="D17" s="21">
-        <v>9.8999999999999999E-4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
+      <c r="D19" s="20">
+        <v>9.8999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
         <v>1341</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B20" s="10" t="s">
         <v>1365</v>
       </c>
-      <c r="C18" s="21">
+      <c r="C20" s="20">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="D18" s="21">
-        <v>1.2899999999999999E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
+      <c r="D20" s="20">
+        <v>1.2899999999999999E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
         <v>1342</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B21" s="10" t="s">
         <v>1366</v>
       </c>
-      <c r="C19" s="21">
+      <c r="C21" s="20">
         <v>1.952E-3</v>
       </c>
-      <c r="D19" s="21">
-        <v>1.951E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
+      <c r="D21" s="20">
+        <v>1.951E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
         <v>1343</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B22" s="10" t="s">
         <v>1369</v>
       </c>
-      <c r="C20" s="21">
+      <c r="C22" s="20">
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="D20" s="21">
-        <v>1.6900000000000001E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="s">
+      <c r="D22" s="20">
+        <v>1.6900000000000001E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
         <v>1344</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B23" s="10" t="s">
         <v>1367</v>
       </c>
-      <c r="C21" s="21">
+      <c r="C23" s="20">
         <v>1.66E-4</v>
       </c>
-      <c r="D21" s="21">
-        <v>1.65E-4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
+      <c r="D23" s="20">
+        <v>1.65E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
         <v>1345</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B24" s="10" t="s">
         <v>1368</v>
       </c>
-      <c r="C22" s="21">
+      <c r="C24" s="20">
         <v>1E-3</v>
       </c>
-      <c r="D22" s="21">
+      <c r="D24" s="20">
         <v>9.8999999999999999E-4</v>
       </c>
     </row>
@@ -5633,10 +5811,4093 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S69"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="15.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="15.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="15.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="15.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B1" s="26" t="s">
+        <v>1374</v>
+      </c>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27" t="s">
+        <v>1375</v>
+      </c>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="26" t="s">
+        <v>1376</v>
+      </c>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="27" t="s">
+        <v>1377</v>
+      </c>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="26" t="s">
+        <v>1378</v>
+      </c>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="27" t="s">
+        <v>1379</v>
+      </c>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>1221</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>1380</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>1381</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>1382</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>1380</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>1381</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>1382</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>1380</v>
+      </c>
+      <c r="I2" s="30" t="s">
+        <v>1381</v>
+      </c>
+      <c r="J2" s="29" t="s">
+        <v>1382</v>
+      </c>
+      <c r="K2" s="31" t="s">
+        <v>1380</v>
+      </c>
+      <c r="L2" s="32" t="s">
+        <v>1381</v>
+      </c>
+      <c r="M2" s="31" t="s">
+        <v>1382</v>
+      </c>
+      <c r="N2" s="29" t="s">
+        <v>1380</v>
+      </c>
+      <c r="O2" s="30" t="s">
+        <v>1381</v>
+      </c>
+      <c r="P2" s="29" t="s">
+        <v>1382</v>
+      </c>
+      <c r="Q2" s="31" t="s">
+        <v>1380</v>
+      </c>
+      <c r="R2" s="32" t="s">
+        <v>1381</v>
+      </c>
+      <c r="S2" s="31" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="33">
+        <v>0.37130000000000002</v>
+      </c>
+      <c r="C3" s="34">
+        <v>25</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E3" s="35">
+        <v>1</v>
+      </c>
+      <c r="F3" s="35">
+        <v>24</v>
+      </c>
+      <c r="G3" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H3" s="36">
+        <v>0.56389999999999996</v>
+      </c>
+      <c r="I3" s="37">
+        <v>24</v>
+      </c>
+      <c r="J3" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K3" s="35">
+        <v>1</v>
+      </c>
+      <c r="L3" s="35">
+        <v>25</v>
+      </c>
+      <c r="M3" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N3" s="37">
+        <v>1</v>
+      </c>
+      <c r="O3" s="37">
+        <v>25</v>
+      </c>
+      <c r="P3" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q3" s="38">
+        <v>0.59689999999999999</v>
+      </c>
+      <c r="R3" s="35">
+        <v>25</v>
+      </c>
+      <c r="S3" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>1384</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="H4" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="I4" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="J4" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="K4" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="L4" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="M4" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="N4" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="O4" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="P4" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="Q4" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="R4" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="S4" s="28" t="s">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="33">
+        <v>1</v>
+      </c>
+      <c r="C5" s="34">
+        <v>19</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E5" s="38">
+        <v>0.126</v>
+      </c>
+      <c r="F5" s="35">
+        <v>16</v>
+      </c>
+      <c r="G5" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H5" s="36">
+        <v>0.37140000000000001</v>
+      </c>
+      <c r="I5" s="37">
+        <v>16</v>
+      </c>
+      <c r="J5" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K5" s="35">
+        <v>1</v>
+      </c>
+      <c r="L5" s="35">
+        <v>19</v>
+      </c>
+      <c r="M5" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N5" s="36">
+        <v>0.98040000000000005</v>
+      </c>
+      <c r="O5" s="37">
+        <v>19</v>
+      </c>
+      <c r="P5" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q5" s="35">
+        <v>1</v>
+      </c>
+      <c r="R5" s="35">
+        <v>19</v>
+      </c>
+      <c r="S5" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="33">
+        <v>1</v>
+      </c>
+      <c r="C6" s="34">
+        <v>21</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E6" s="38">
+        <v>0.39910000000000001</v>
+      </c>
+      <c r="F6" s="35">
+        <v>21</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H6" s="36">
+        <v>8.6770000000000007E-3</v>
+      </c>
+      <c r="I6" s="37">
+        <v>21</v>
+      </c>
+      <c r="J6" s="39">
+        <v>5.1745000000000003E-3</v>
+      </c>
+      <c r="K6" s="38">
+        <v>0.52569999999999995</v>
+      </c>
+      <c r="L6" s="35">
+        <v>21</v>
+      </c>
+      <c r="M6" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N6" s="36">
+        <v>0.2863</v>
+      </c>
+      <c r="O6" s="37">
+        <v>21</v>
+      </c>
+      <c r="P6" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q6" s="35">
+        <v>1</v>
+      </c>
+      <c r="R6" s="35">
+        <v>21</v>
+      </c>
+      <c r="S6" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="B7" s="33">
+        <v>1</v>
+      </c>
+      <c r="C7" s="34">
+        <v>12</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E7" s="35">
+        <v>1</v>
+      </c>
+      <c r="F7" s="35">
+        <v>12</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H7" s="36">
+        <v>8.4110000000000004E-2</v>
+      </c>
+      <c r="I7" s="37">
+        <v>12</v>
+      </c>
+      <c r="J7" s="37">
+        <v>-2.5000000000000001E-3</v>
+      </c>
+      <c r="K7" s="35">
+        <v>1</v>
+      </c>
+      <c r="L7" s="35">
+        <v>12</v>
+      </c>
+      <c r="M7" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N7" s="36">
+        <v>0.15770000000000001</v>
+      </c>
+      <c r="O7" s="37">
+        <v>12</v>
+      </c>
+      <c r="P7" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q7" s="38">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="R7" s="35">
+        <v>12</v>
+      </c>
+      <c r="S7" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="B8" s="33">
+        <v>1</v>
+      </c>
+      <c r="C8" s="34">
+        <v>23</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E8" s="38">
+        <v>8.3479999999999999E-2</v>
+      </c>
+      <c r="F8" s="35">
+        <v>23</v>
+      </c>
+      <c r="G8" s="40">
+        <v>5.7099999999999998E-3</v>
+      </c>
+      <c r="H8" s="36">
+        <v>2.5680000000000001E-2</v>
+      </c>
+      <c r="I8" s="37">
+        <v>23</v>
+      </c>
+      <c r="J8" s="36">
+        <v>1.1949E-2</v>
+      </c>
+      <c r="K8" s="38">
+        <v>0.59989999999999999</v>
+      </c>
+      <c r="L8" s="35">
+        <v>23</v>
+      </c>
+      <c r="M8" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N8" s="37">
+        <v>1</v>
+      </c>
+      <c r="O8" s="37">
+        <v>23</v>
+      </c>
+      <c r="P8" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q8" s="38">
+        <v>0.15740000000000001</v>
+      </c>
+      <c r="R8" s="35">
+        <v>23</v>
+      </c>
+      <c r="S8" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B9" s="33">
+        <v>0.37130000000000002</v>
+      </c>
+      <c r="C9" s="34">
+        <v>16</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E9" s="38">
+        <v>0.46949999999999997</v>
+      </c>
+      <c r="F9" s="35">
+        <v>16</v>
+      </c>
+      <c r="G9" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H9" s="36">
+        <v>4.8180000000000001E-2</v>
+      </c>
+      <c r="I9" s="37">
+        <v>16</v>
+      </c>
+      <c r="J9" s="39">
+        <v>9.1489999999999991E-3</v>
+      </c>
+      <c r="K9" s="38">
+        <v>8.3720000000000003E-2</v>
+      </c>
+      <c r="L9" s="35">
+        <v>16</v>
+      </c>
+      <c r="M9" s="40">
+        <v>8.0099999999999998E-3</v>
+      </c>
+      <c r="N9" s="36">
+        <v>0.61729999999999996</v>
+      </c>
+      <c r="O9" s="37">
+        <v>16</v>
+      </c>
+      <c r="P9" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q9" s="38">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="R9" s="35">
+        <v>16</v>
+      </c>
+      <c r="S9" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B10" s="33">
+        <v>1</v>
+      </c>
+      <c r="C10" s="34">
+        <v>18</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E10" s="38">
+        <v>0.2006</v>
+      </c>
+      <c r="F10" s="35">
+        <v>18</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H10" s="36">
+        <v>0.33739999999999998</v>
+      </c>
+      <c r="I10" s="37">
+        <v>18</v>
+      </c>
+      <c r="J10" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K10" s="38">
+        <v>0.63</v>
+      </c>
+      <c r="L10" s="35">
+        <v>18</v>
+      </c>
+      <c r="M10" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N10" s="37">
+        <v>1</v>
+      </c>
+      <c r="O10" s="37">
+        <v>18</v>
+      </c>
+      <c r="P10" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q10" s="38">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="R10" s="35">
+        <v>18</v>
+      </c>
+      <c r="S10" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B11" s="33">
+        <v>1</v>
+      </c>
+      <c r="C11" s="34">
+        <v>30</v>
+      </c>
+      <c r="D11" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E11" s="38">
+        <v>0.81389999999999996</v>
+      </c>
+      <c r="F11" s="35">
+        <v>30</v>
+      </c>
+      <c r="G11" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H11" s="36">
+        <v>1.984E-2</v>
+      </c>
+      <c r="I11" s="37">
+        <v>30</v>
+      </c>
+      <c r="J11" s="39">
+        <v>9.2490000000000003E-3</v>
+      </c>
+      <c r="K11" s="38">
+        <v>0.30930000000000002</v>
+      </c>
+      <c r="L11" s="35">
+        <v>30</v>
+      </c>
+      <c r="M11" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N11" s="37">
+        <v>1</v>
+      </c>
+      <c r="O11" s="37">
+        <v>30</v>
+      </c>
+      <c r="P11" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q11" s="38">
+        <v>0.98089999999999999</v>
+      </c>
+      <c r="R11" s="35">
+        <v>30</v>
+      </c>
+      <c r="S11" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>1386</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="H12" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="I12" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="J12" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="K12" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="L12" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="M12" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="N12" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="O12" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="P12" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="Q12" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="R12" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="S12" s="28" t="s">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>1387</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="H13" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="I13" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="J13" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="K13" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="L13" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="M13" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="N13" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="O13" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="P13" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="Q13" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="R13" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="S13" s="28" t="s">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>1388</v>
+      </c>
+      <c r="B14" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="G14" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="H14" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="I14" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="J14" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="K14" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="L14" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="M14" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="N14" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="O14" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="P14" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="Q14" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="R14" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="S14" s="28" t="s">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>735</v>
+      </c>
+      <c r="B15" s="33">
+        <v>1</v>
+      </c>
+      <c r="C15" s="34">
+        <v>30</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E15" s="38">
+        <v>1.102E-2</v>
+      </c>
+      <c r="F15" s="35">
+        <v>30</v>
+      </c>
+      <c r="G15" s="38">
+        <v>-2.895E-2</v>
+      </c>
+      <c r="H15" s="36">
+        <v>7.6060000000000003E-2</v>
+      </c>
+      <c r="I15" s="37">
+        <v>30</v>
+      </c>
+      <c r="J15" s="36">
+        <v>2.8060000000000002E-2</v>
+      </c>
+      <c r="K15" s="38">
+        <v>0.63149999999999995</v>
+      </c>
+      <c r="L15" s="35">
+        <v>29</v>
+      </c>
+      <c r="M15" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N15" s="36">
+        <v>0.14940000000000001</v>
+      </c>
+      <c r="O15" s="37">
+        <v>30</v>
+      </c>
+      <c r="P15" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q15" s="38">
+        <v>0.15740000000000001</v>
+      </c>
+      <c r="R15" s="35">
+        <v>30</v>
+      </c>
+      <c r="S15" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>741</v>
+      </c>
+      <c r="B16" s="33">
+        <v>1</v>
+      </c>
+      <c r="C16" s="34">
+        <v>30</v>
+      </c>
+      <c r="D16" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E16" s="38">
+        <v>0.39810000000000001</v>
+      </c>
+      <c r="F16" s="35">
+        <v>30</v>
+      </c>
+      <c r="G16" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H16" s="36">
+        <v>1.6660000000000001E-2</v>
+      </c>
+      <c r="I16" s="37">
+        <v>30</v>
+      </c>
+      <c r="J16" s="36">
+        <v>1.2489999999999999E-2</v>
+      </c>
+      <c r="K16" s="38">
+        <v>0.98089999999999999</v>
+      </c>
+      <c r="L16" s="35">
+        <v>30</v>
+      </c>
+      <c r="M16" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N16" s="36">
+        <v>0.10630000000000001</v>
+      </c>
+      <c r="O16" s="37">
+        <v>30</v>
+      </c>
+      <c r="P16" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q16" s="38">
+        <v>2.5530000000000001E-2</v>
+      </c>
+      <c r="R16" s="35">
+        <v>30</v>
+      </c>
+      <c r="S16" s="38">
+        <v>-5.9899999999999995E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B17" s="33">
+        <v>1</v>
+      </c>
+      <c r="C17" s="34">
+        <v>19</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E17" s="38">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="F17" s="35">
+        <v>19</v>
+      </c>
+      <c r="G17" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H17" s="36">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="I17" s="37">
+        <v>19</v>
+      </c>
+      <c r="J17" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K17" s="35">
+        <v>1</v>
+      </c>
+      <c r="L17" s="35">
+        <v>19</v>
+      </c>
+      <c r="M17" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N17" s="36">
+        <v>5.1419999999999999E-3</v>
+      </c>
+      <c r="O17" s="37">
+        <v>19</v>
+      </c>
+      <c r="P17" s="36">
+        <v>-1.4200000000000001E-2</v>
+      </c>
+      <c r="Q17" s="35">
+        <v>1</v>
+      </c>
+      <c r="R17" s="35">
+        <v>19</v>
+      </c>
+      <c r="S17" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>1389</v>
+      </c>
+      <c r="B18" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="F18" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="G18" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="H18" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="I18" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="J18" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="K18" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="L18" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="M18" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="N18" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="O18" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="P18" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="Q18" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="R18" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="S18" s="28" t="s">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>702</v>
+      </c>
+      <c r="B19" s="33">
+        <v>1</v>
+      </c>
+      <c r="C19" s="34">
+        <v>13</v>
+      </c>
+      <c r="D19" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E19" s="38">
+        <v>0.86260000000000003</v>
+      </c>
+      <c r="F19" s="35">
+        <v>13</v>
+      </c>
+      <c r="G19" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H19" s="36">
+        <v>0.6038</v>
+      </c>
+      <c r="I19" s="37">
+        <v>13</v>
+      </c>
+      <c r="J19" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K19" s="35">
+        <v>1</v>
+      </c>
+      <c r="L19" s="35">
+        <v>13</v>
+      </c>
+      <c r="M19" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N19" s="36">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="O19" s="37">
+        <v>13</v>
+      </c>
+      <c r="P19" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q19" s="38">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="R19" s="35">
+        <v>13</v>
+      </c>
+      <c r="S19" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="B20" s="33">
+        <v>1</v>
+      </c>
+      <c r="C20" s="34">
+        <v>30</v>
+      </c>
+      <c r="D20" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E20" s="38">
+        <v>0.89849999999999997</v>
+      </c>
+      <c r="F20" s="35">
+        <v>30</v>
+      </c>
+      <c r="G20" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H20" s="36">
+        <v>0.19739999999999999</v>
+      </c>
+      <c r="I20" s="37">
+        <v>30</v>
+      </c>
+      <c r="J20" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K20" s="38">
+        <v>0.15740000000000001</v>
+      </c>
+      <c r="L20" s="35">
+        <v>30</v>
+      </c>
+      <c r="M20" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N20" s="36">
+        <v>0.15740000000000001</v>
+      </c>
+      <c r="O20" s="37">
+        <v>30</v>
+      </c>
+      <c r="P20" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q20" s="35">
+        <v>1</v>
+      </c>
+      <c r="R20" s="35">
+        <v>30</v>
+      </c>
+      <c r="S20" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>813</v>
+      </c>
+      <c r="B21" s="33">
+        <v>1</v>
+      </c>
+      <c r="C21" s="34">
+        <v>29</v>
+      </c>
+      <c r="D21" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E21" s="35">
+        <v>1</v>
+      </c>
+      <c r="F21" s="35">
+        <v>29</v>
+      </c>
+      <c r="G21" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H21" s="36">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="I21" s="37">
+        <v>29</v>
+      </c>
+      <c r="J21" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K21" s="38">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="L21" s="35">
+        <v>29</v>
+      </c>
+      <c r="M21" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N21" s="37">
+        <v>1</v>
+      </c>
+      <c r="O21" s="37">
+        <v>29</v>
+      </c>
+      <c r="P21" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q21" s="35">
+        <v>1</v>
+      </c>
+      <c r="R21" s="35">
+        <v>29</v>
+      </c>
+      <c r="S21" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>759</v>
+      </c>
+      <c r="B22" s="33">
+        <v>1</v>
+      </c>
+      <c r="C22" s="34">
+        <v>27</v>
+      </c>
+      <c r="D22" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E22" s="35">
+        <v>1</v>
+      </c>
+      <c r="F22" s="35">
+        <v>27</v>
+      </c>
+      <c r="G22" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H22" s="36">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="I22" s="37">
+        <v>27</v>
+      </c>
+      <c r="J22" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K22" s="35">
+        <v>1</v>
+      </c>
+      <c r="L22" s="35">
+        <v>27</v>
+      </c>
+      <c r="M22" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N22" s="37">
+        <v>1</v>
+      </c>
+      <c r="O22" s="37">
+        <v>27</v>
+      </c>
+      <c r="P22" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q22" s="35">
+        <v>1</v>
+      </c>
+      <c r="R22" s="35">
+        <v>27</v>
+      </c>
+      <c r="S22" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="B23" s="33">
+        <v>0.65549999999999997</v>
+      </c>
+      <c r="C23" s="34">
+        <v>22</v>
+      </c>
+      <c r="D23" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E23" s="38">
+        <v>0.1075</v>
+      </c>
+      <c r="F23" s="35">
+        <v>27</v>
+      </c>
+      <c r="G23" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H23" s="36">
+        <v>0.1186</v>
+      </c>
+      <c r="I23" s="37">
+        <v>27</v>
+      </c>
+      <c r="J23" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K23" s="38">
+        <v>7.9119999999999996E-2</v>
+      </c>
+      <c r="L23" s="35">
+        <v>27</v>
+      </c>
+      <c r="M23" s="35">
+        <v>-8.6E-3</v>
+      </c>
+      <c r="N23" s="36">
+        <v>0.16650000000000001</v>
+      </c>
+      <c r="O23" s="37">
+        <v>27</v>
+      </c>
+      <c r="P23" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q23" s="38">
+        <v>0.2102</v>
+      </c>
+      <c r="R23" s="35">
+        <v>27</v>
+      </c>
+      <c r="S23" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>537</v>
+      </c>
+      <c r="B24" s="33">
+        <v>1</v>
+      </c>
+      <c r="C24" s="34">
+        <v>24</v>
+      </c>
+      <c r="D24" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E24" s="38">
+        <v>0.32879999999999998</v>
+      </c>
+      <c r="F24" s="35">
+        <v>24</v>
+      </c>
+      <c r="G24" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H24" s="36">
+        <v>0.1678</v>
+      </c>
+      <c r="I24" s="37">
+        <v>24</v>
+      </c>
+      <c r="J24" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K24" s="38">
+        <v>0.74550000000000005</v>
+      </c>
+      <c r="L24" s="35">
+        <v>24</v>
+      </c>
+      <c r="M24" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N24" s="36">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="O24" s="37">
+        <v>19</v>
+      </c>
+      <c r="P24" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q24" s="38">
+        <v>8.3460000000000006E-2</v>
+      </c>
+      <c r="R24" s="35">
+        <v>24</v>
+      </c>
+      <c r="S24" s="38">
+        <v>-1.251E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>649</v>
+      </c>
+      <c r="B25" s="33">
+        <v>1</v>
+      </c>
+      <c r="C25" s="34">
+        <v>29</v>
+      </c>
+      <c r="D25" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E25" s="38">
+        <v>2.555E-2</v>
+      </c>
+      <c r="F25" s="35">
+        <v>29</v>
+      </c>
+      <c r="G25" s="40">
+        <v>-2.0100000000000001E-3</v>
+      </c>
+      <c r="H25" s="36">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="I25" s="37">
+        <v>29</v>
+      </c>
+      <c r="J25" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K25" s="35">
+        <v>1</v>
+      </c>
+      <c r="L25" s="35">
+        <v>29</v>
+      </c>
+      <c r="M25" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N25" s="36">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="O25" s="37">
+        <v>29</v>
+      </c>
+      <c r="P25" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q25" s="38">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="R25" s="35">
+        <v>29</v>
+      </c>
+      <c r="S25" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>1390</v>
+      </c>
+      <c r="B26" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C26" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="D26" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="E26" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="F26" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="G26" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="H26" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="I26" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="J26" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="K26" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="L26" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="M26" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="N26" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="O26" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="P26" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="Q26" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="R26" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="S26" s="28" t="s">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="B27" s="33">
+        <v>0.35899999999999999</v>
+      </c>
+      <c r="C27" s="34">
+        <v>20</v>
+      </c>
+      <c r="D27" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E27" s="38">
+        <v>3.2070000000000001E-2</v>
+      </c>
+      <c r="F27" s="35">
+        <v>20</v>
+      </c>
+      <c r="G27" s="38">
+        <v>1.6209999999999999E-2</v>
+      </c>
+      <c r="H27" s="36">
+        <v>1.0359999999999999E-2</v>
+      </c>
+      <c r="I27" s="37">
+        <v>20</v>
+      </c>
+      <c r="J27" s="36">
+        <v>1.0848999999999999E-2</v>
+      </c>
+      <c r="K27" s="38">
+        <v>0.1011</v>
+      </c>
+      <c r="L27" s="35">
+        <v>20</v>
+      </c>
+      <c r="M27" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N27" s="36">
+        <v>0.20219999999999999</v>
+      </c>
+      <c r="O27" s="37">
+        <v>20</v>
+      </c>
+      <c r="P27" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q27" s="38">
+        <v>0.60580000000000001</v>
+      </c>
+      <c r="R27" s="35">
+        <v>20</v>
+      </c>
+      <c r="S27" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>1391</v>
+      </c>
+      <c r="B28" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C28" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="D28" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="E28" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="F28" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="G28" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="H28" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="I28" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="J28" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="K28" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="L28" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="M28" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="N28" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="O28" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="P28" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="Q28" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="R28" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="S28" s="28" t="s">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>777</v>
+      </c>
+      <c r="B29" s="33">
+        <v>1</v>
+      </c>
+      <c r="C29" s="34">
+        <v>20</v>
+      </c>
+      <c r="D29" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E29" s="38">
+        <v>0.60819999999999996</v>
+      </c>
+      <c r="F29" s="35">
+        <v>19</v>
+      </c>
+      <c r="G29" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H29" s="36">
+        <v>0.56410000000000005</v>
+      </c>
+      <c r="I29" s="37">
+        <v>19</v>
+      </c>
+      <c r="J29" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K29" s="35">
+        <v>1</v>
+      </c>
+      <c r="L29" s="35">
+        <v>19</v>
+      </c>
+      <c r="M29" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N29" s="37">
+        <v>1</v>
+      </c>
+      <c r="O29" s="37">
+        <v>20</v>
+      </c>
+      <c r="P29" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q29" s="35">
+        <v>1</v>
+      </c>
+      <c r="R29" s="35">
+        <v>20</v>
+      </c>
+      <c r="S29" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>931</v>
+      </c>
+      <c r="B30" s="33">
+        <v>1</v>
+      </c>
+      <c r="C30" s="34">
+        <v>22</v>
+      </c>
+      <c r="D30" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E30" s="38">
+        <v>0.28539999999999999</v>
+      </c>
+      <c r="F30" s="35">
+        <v>23</v>
+      </c>
+      <c r="G30" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H30" s="36">
+        <v>0.59530000000000005</v>
+      </c>
+      <c r="I30" s="37">
+        <v>23</v>
+      </c>
+      <c r="J30" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K30" s="35">
+        <v>1</v>
+      </c>
+      <c r="L30" s="35">
+        <v>23</v>
+      </c>
+      <c r="M30" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N30" s="37">
+        <v>1</v>
+      </c>
+      <c r="O30" s="37">
+        <v>23</v>
+      </c>
+      <c r="P30" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q30" s="38">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="R30" s="35">
+        <v>23</v>
+      </c>
+      <c r="S30" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="B31" s="33">
+        <v>0.37130000000000002</v>
+      </c>
+      <c r="C31" s="34">
+        <v>27</v>
+      </c>
+      <c r="D31" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E31" s="38">
+        <v>0.59430000000000005</v>
+      </c>
+      <c r="F31" s="35">
+        <v>27</v>
+      </c>
+      <c r="G31" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H31" s="36">
+        <v>4.48E-2</v>
+      </c>
+      <c r="I31" s="37">
+        <v>27</v>
+      </c>
+      <c r="J31" s="39">
+        <v>2.7989999999999998E-3</v>
+      </c>
+      <c r="K31" s="38">
+        <v>1.453E-2</v>
+      </c>
+      <c r="L31" s="35">
+        <v>27</v>
+      </c>
+      <c r="M31" s="40">
+        <v>2.3500000000000001E-3</v>
+      </c>
+      <c r="N31" s="36">
+        <v>0.97870000000000001</v>
+      </c>
+      <c r="O31" s="37">
+        <v>27</v>
+      </c>
+      <c r="P31" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q31" s="38">
+        <v>0.15740000000000001</v>
+      </c>
+      <c r="R31" s="35">
+        <v>27</v>
+      </c>
+      <c r="S31" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="B32" s="33">
+        <v>1</v>
+      </c>
+      <c r="C32" s="34">
+        <v>16</v>
+      </c>
+      <c r="D32" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E32" s="38">
+        <v>0.30230000000000001</v>
+      </c>
+      <c r="F32" s="35">
+        <v>16</v>
+      </c>
+      <c r="G32" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H32" s="36">
+        <v>0.97609999999999997</v>
+      </c>
+      <c r="I32" s="37">
+        <v>16</v>
+      </c>
+      <c r="J32" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K32" s="35">
+        <v>1</v>
+      </c>
+      <c r="L32" s="35">
+        <v>16</v>
+      </c>
+      <c r="M32" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N32" s="37">
+        <v>1</v>
+      </c>
+      <c r="O32" s="37">
+        <v>16</v>
+      </c>
+      <c r="P32" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q32" s="38">
+        <v>8.3720000000000003E-2</v>
+      </c>
+      <c r="R32" s="35">
+        <v>16</v>
+      </c>
+      <c r="S32" s="40">
+        <v>-1.7100000000000001E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="B33" s="33">
+        <v>0.37130000000000002</v>
+      </c>
+      <c r="C33" s="34">
+        <v>19</v>
+      </c>
+      <c r="D33" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E33" s="38">
+        <v>2.5860000000000001E-2</v>
+      </c>
+      <c r="F33" s="35">
+        <v>19</v>
+      </c>
+      <c r="G33" s="40">
+        <v>4.4099999999999999E-3</v>
+      </c>
+      <c r="H33" s="36">
+        <v>8.6569999999999998E-3</v>
+      </c>
+      <c r="I33" s="37">
+        <v>19</v>
+      </c>
+      <c r="J33" s="36">
+        <v>1.2049000000000001E-2</v>
+      </c>
+      <c r="K33" s="38">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="L33" s="35">
+        <v>19</v>
+      </c>
+      <c r="M33" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N33" s="37">
+        <v>1</v>
+      </c>
+      <c r="O33" s="37">
+        <v>19</v>
+      </c>
+      <c r="P33" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q33" s="38">
+        <v>1.4829999999999999E-2</v>
+      </c>
+      <c r="R33" s="35">
+        <v>19</v>
+      </c>
+      <c r="S33" s="38">
+        <v>-4.0855000000000002E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>463</v>
+      </c>
+      <c r="B34" s="33">
+        <v>1</v>
+      </c>
+      <c r="C34" s="34">
+        <v>23</v>
+      </c>
+      <c r="D34" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E34" s="38">
+        <v>1.004E-2</v>
+      </c>
+      <c r="F34" s="35">
+        <v>23</v>
+      </c>
+      <c r="G34" s="38">
+        <v>-2.3599999999999999E-2</v>
+      </c>
+      <c r="H34" s="36">
+        <v>8.0400000000000003E-3</v>
+      </c>
+      <c r="I34" s="37">
+        <v>23</v>
+      </c>
+      <c r="J34" s="36">
+        <v>-6.1249999999999999E-2</v>
+      </c>
+      <c r="K34" s="38">
+        <v>0.65580000000000005</v>
+      </c>
+      <c r="L34" s="35">
+        <v>23</v>
+      </c>
+      <c r="M34" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N34" s="36">
+        <v>8.5220000000000004E-2</v>
+      </c>
+      <c r="O34" s="37">
+        <v>23</v>
+      </c>
+      <c r="P34" s="39">
+        <v>-5.8349999999999999E-3</v>
+      </c>
+      <c r="Q34" s="38">
+        <v>1.088E-3</v>
+      </c>
+      <c r="R34" s="35">
+        <v>23</v>
+      </c>
+      <c r="S34" s="40">
+        <v>-8.7100000000000007E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>1199</v>
+      </c>
+      <c r="B35" s="33">
+        <v>4.5900000000000003E-2</v>
+      </c>
+      <c r="C35" s="34">
+        <v>18</v>
+      </c>
+      <c r="D35" s="33">
+        <v>0</v>
+      </c>
+      <c r="E35" s="38">
+        <v>0.1898</v>
+      </c>
+      <c r="F35" s="35">
+        <v>18</v>
+      </c>
+      <c r="G35" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H35" s="36">
+        <v>5.1479999999999998E-2</v>
+      </c>
+      <c r="I35" s="37">
+        <v>18</v>
+      </c>
+      <c r="J35" s="37">
+        <v>6.8999999999999999E-3</v>
+      </c>
+      <c r="K35" s="38">
+        <v>0.17130000000000001</v>
+      </c>
+      <c r="L35" s="35">
+        <v>18</v>
+      </c>
+      <c r="M35" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N35" s="36">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="O35" s="37">
+        <v>18</v>
+      </c>
+      <c r="P35" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q35" s="35">
+        <v>1</v>
+      </c>
+      <c r="R35" s="35">
+        <v>18</v>
+      </c>
+      <c r="S35" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B36" s="33">
+        <v>1</v>
+      </c>
+      <c r="C36" s="34">
+        <v>24</v>
+      </c>
+      <c r="D36" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E36" s="38">
+        <v>0.20849999999999999</v>
+      </c>
+      <c r="F36" s="35">
+        <v>24</v>
+      </c>
+      <c r="G36" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H36" s="36">
+        <v>2.5649999999999999E-2</v>
+      </c>
+      <c r="I36" s="37">
+        <v>24</v>
+      </c>
+      <c r="J36" s="39">
+        <v>8.9490000000000004E-3</v>
+      </c>
+      <c r="K36" s="38">
+        <v>8.3460000000000006E-2</v>
+      </c>
+      <c r="L36" s="35">
+        <v>24</v>
+      </c>
+      <c r="M36" s="40">
+        <v>3.81E-3</v>
+      </c>
+      <c r="N36" s="37">
+        <v>1</v>
+      </c>
+      <c r="O36" s="37">
+        <v>24</v>
+      </c>
+      <c r="P36" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q36" s="38">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="R36" s="35">
+        <v>24</v>
+      </c>
+      <c r="S36" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B37" s="33">
+        <v>1</v>
+      </c>
+      <c r="C37" s="34">
+        <v>24</v>
+      </c>
+      <c r="D37" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E37" s="38">
+        <v>8.3460000000000006E-2</v>
+      </c>
+      <c r="F37" s="35">
+        <v>24</v>
+      </c>
+      <c r="G37" s="40">
+        <v>4.6100000000000004E-3</v>
+      </c>
+      <c r="H37" s="36">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="I37" s="37">
+        <v>24</v>
+      </c>
+      <c r="J37" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K37" s="38">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="L37" s="35">
+        <v>24</v>
+      </c>
+      <c r="M37" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N37" s="36">
+        <v>0.83809999999999996</v>
+      </c>
+      <c r="O37" s="37">
+        <v>24</v>
+      </c>
+      <c r="P37" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q37" s="38">
+        <v>0.65539999999999998</v>
+      </c>
+      <c r="R37" s="35">
+        <v>24</v>
+      </c>
+      <c r="S37" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="B38" s="33">
+        <v>1</v>
+      </c>
+      <c r="C38" s="34">
+        <v>12</v>
+      </c>
+      <c r="D38" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E38" s="35">
+        <v>1</v>
+      </c>
+      <c r="F38" s="35">
+        <v>12</v>
+      </c>
+      <c r="G38" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H38" s="37">
+        <v>1</v>
+      </c>
+      <c r="I38" s="37">
+        <v>12</v>
+      </c>
+      <c r="J38" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K38" s="38">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="L38" s="35">
+        <v>12</v>
+      </c>
+      <c r="M38" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N38" s="37">
+        <v>1</v>
+      </c>
+      <c r="O38" s="37">
+        <v>12</v>
+      </c>
+      <c r="P38" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q38" s="35">
+        <v>1</v>
+      </c>
+      <c r="R38" s="35">
+        <v>12</v>
+      </c>
+      <c r="S38" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>1392</v>
+      </c>
+      <c r="B39" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C39" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="D39" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="E39" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="F39" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="G39" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="H39" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="I39" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="J39" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="K39" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="L39" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="M39" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="N39" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="O39" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="P39" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="Q39" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="R39" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="S39" s="28" t="s">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>515</v>
+      </c>
+      <c r="B40" s="33">
+        <v>1</v>
+      </c>
+      <c r="C40" s="34">
+        <v>21</v>
+      </c>
+      <c r="D40" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E40" s="38">
+        <v>7.9089999999999994E-2</v>
+      </c>
+      <c r="F40" s="35">
+        <v>21</v>
+      </c>
+      <c r="G40" s="40">
+        <v>-1.48E-3</v>
+      </c>
+      <c r="H40" s="36">
+        <v>0.60250000000000004</v>
+      </c>
+      <c r="I40" s="37">
+        <v>21</v>
+      </c>
+      <c r="J40" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K40" s="38">
+        <v>0.79579999999999995</v>
+      </c>
+      <c r="L40" s="35">
+        <v>21</v>
+      </c>
+      <c r="M40" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N40" s="37">
+        <v>1</v>
+      </c>
+      <c r="O40" s="37">
+        <v>21</v>
+      </c>
+      <c r="P40" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q40" s="35">
+        <v>1</v>
+      </c>
+      <c r="R40" s="35">
+        <v>21</v>
+      </c>
+      <c r="S40" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="B41" s="33">
+        <v>1</v>
+      </c>
+      <c r="C41" s="34">
+        <v>18</v>
+      </c>
+      <c r="D41" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E41" s="38">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F41" s="35">
+        <v>18</v>
+      </c>
+      <c r="G41" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H41" s="36">
+        <v>3.1749999999999999E-3</v>
+      </c>
+      <c r="I41" s="37">
+        <v>18</v>
+      </c>
+      <c r="J41" s="39">
+        <v>9.8490000000000001E-3</v>
+      </c>
+      <c r="K41" s="38">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="L41" s="35">
+        <v>18</v>
+      </c>
+      <c r="M41" s="40">
+        <v>4.6099999999999995E-3</v>
+      </c>
+      <c r="N41" s="36">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="O41" s="37">
+        <v>18</v>
+      </c>
+      <c r="P41" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q41" s="35">
+        <v>1</v>
+      </c>
+      <c r="R41" s="35">
+        <v>18</v>
+      </c>
+      <c r="S41" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="B42" s="33">
+        <v>1</v>
+      </c>
+      <c r="C42" s="34">
+        <v>28</v>
+      </c>
+      <c r="D42" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E42" s="38">
+        <v>0.56389999999999996</v>
+      </c>
+      <c r="F42" s="35">
+        <v>28</v>
+      </c>
+      <c r="G42" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H42" s="36">
+        <v>0.17680000000000001</v>
+      </c>
+      <c r="I42" s="37">
+        <v>28</v>
+      </c>
+      <c r="J42" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K42" s="38">
+        <v>0.20369999999999999</v>
+      </c>
+      <c r="L42" s="35">
+        <v>28</v>
+      </c>
+      <c r="M42" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N42" s="36">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="O42" s="37">
+        <v>28</v>
+      </c>
+      <c r="P42" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q42" s="38">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="R42" s="35">
+        <v>28</v>
+      </c>
+      <c r="S42" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="B43" s="33">
+        <v>1</v>
+      </c>
+      <c r="C43" s="34">
+        <v>23</v>
+      </c>
+      <c r="D43" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E43" s="35">
+        <v>1</v>
+      </c>
+      <c r="F43" s="35">
+        <v>23</v>
+      </c>
+      <c r="G43" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H43" s="36">
+        <v>2.0040000000000001E-3</v>
+      </c>
+      <c r="I43" s="37">
+        <v>23</v>
+      </c>
+      <c r="J43" s="37">
+        <v>9.1000000000000004E-3</v>
+      </c>
+      <c r="K43" s="38">
+        <v>0.90159999999999996</v>
+      </c>
+      <c r="L43" s="35">
+        <v>23</v>
+      </c>
+      <c r="M43" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N43" s="36">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="O43" s="37">
+        <v>23</v>
+      </c>
+      <c r="P43" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q43" s="38">
+        <v>0.21</v>
+      </c>
+      <c r="R43" s="35">
+        <v>23</v>
+      </c>
+      <c r="S43" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="B44" s="33">
+        <v>1</v>
+      </c>
+      <c r="C44" s="34">
+        <v>14</v>
+      </c>
+      <c r="D44" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E44" s="38">
+        <v>8.387E-2</v>
+      </c>
+      <c r="F44" s="35">
+        <v>14</v>
+      </c>
+      <c r="G44" s="35">
+        <v>4.1999999999999997E-3</v>
+      </c>
+      <c r="H44" s="36">
+        <v>8.387E-2</v>
+      </c>
+      <c r="I44" s="37">
+        <v>14</v>
+      </c>
+      <c r="J44" s="37">
+        <v>9.7000000000000003E-3</v>
+      </c>
+      <c r="K44" s="38">
+        <v>0.95830000000000004</v>
+      </c>
+      <c r="L44" s="35">
+        <v>14</v>
+      </c>
+      <c r="M44" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N44" s="36">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="O44" s="37">
+        <v>14</v>
+      </c>
+      <c r="P44" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q44" s="38">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="R44" s="35">
+        <v>14</v>
+      </c>
+      <c r="S44" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="B45" s="33">
+        <v>1</v>
+      </c>
+      <c r="C45" s="34">
+        <v>18</v>
+      </c>
+      <c r="D45" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E45" s="38">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="F45" s="35">
+        <v>18</v>
+      </c>
+      <c r="G45" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H45" s="36">
+        <v>8.362E-2</v>
+      </c>
+      <c r="I45" s="37">
+        <v>18</v>
+      </c>
+      <c r="J45" s="37">
+        <v>-7.1000000000000004E-3</v>
+      </c>
+      <c r="K45" s="38">
+        <v>0.74539999999999995</v>
+      </c>
+      <c r="L45" s="35">
+        <v>18</v>
+      </c>
+      <c r="M45" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N45" s="36">
+        <v>0.1575</v>
+      </c>
+      <c r="O45" s="37">
+        <v>18</v>
+      </c>
+      <c r="P45" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q45" s="35">
+        <v>1</v>
+      </c>
+      <c r="R45" s="35">
+        <v>18</v>
+      </c>
+      <c r="S45" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="B46" s="33">
+        <v>0.96579999999999999</v>
+      </c>
+      <c r="C46" s="34">
+        <v>17</v>
+      </c>
+      <c r="D46" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E46" s="38">
+        <v>0.66890000000000005</v>
+      </c>
+      <c r="F46" s="35">
+        <v>17</v>
+      </c>
+      <c r="G46" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H46" s="36">
+        <v>0.94869999999999999</v>
+      </c>
+      <c r="I46" s="37">
+        <v>17</v>
+      </c>
+      <c r="J46" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K46" s="38">
+        <v>0.11310000000000001</v>
+      </c>
+      <c r="L46" s="35">
+        <v>17</v>
+      </c>
+      <c r="M46" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N46" s="37">
+        <v>1</v>
+      </c>
+      <c r="O46" s="37">
+        <v>17</v>
+      </c>
+      <c r="P46" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q46" s="35">
+        <v>1</v>
+      </c>
+      <c r="R46" s="35">
+        <v>17</v>
+      </c>
+      <c r="S46" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="B47" s="33">
+        <v>1</v>
+      </c>
+      <c r="C47" s="34">
+        <v>19</v>
+      </c>
+      <c r="D47" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E47" s="38">
+        <v>0.54649999999999999</v>
+      </c>
+      <c r="F47" s="35">
+        <v>19</v>
+      </c>
+      <c r="G47" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H47" s="36">
+        <v>0.13039999999999999</v>
+      </c>
+      <c r="I47" s="37">
+        <v>19</v>
+      </c>
+      <c r="J47" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K47" s="38">
+        <v>0.7097</v>
+      </c>
+      <c r="L47" s="35">
+        <v>19</v>
+      </c>
+      <c r="M47" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N47" s="36">
+        <v>0.96950000000000003</v>
+      </c>
+      <c r="O47" s="37">
+        <v>19</v>
+      </c>
+      <c r="P47" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q47" s="38">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="R47" s="35">
+        <v>19</v>
+      </c>
+      <c r="S47" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="B48" s="33">
+        <v>0.97789999999999999</v>
+      </c>
+      <c r="C48" s="34">
+        <v>26</v>
+      </c>
+      <c r="D48" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E48" s="38">
+        <v>0.4047</v>
+      </c>
+      <c r="F48" s="35">
+        <v>26</v>
+      </c>
+      <c r="G48" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H48" s="36">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="I48" s="37">
+        <v>26</v>
+      </c>
+      <c r="J48" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K48" s="38">
+        <v>8.1799999999999998E-3</v>
+      </c>
+      <c r="L48" s="35">
+        <v>26</v>
+      </c>
+      <c r="M48" s="35">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="N48" s="37">
+        <v>1</v>
+      </c>
+      <c r="O48" s="37">
+        <v>26</v>
+      </c>
+      <c r="P48" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q48" s="38">
+        <v>0.56389999999999996</v>
+      </c>
+      <c r="R48" s="35">
+        <v>26</v>
+      </c>
+      <c r="S48" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="B49" s="33">
+        <v>1</v>
+      </c>
+      <c r="C49" s="34">
+        <v>19</v>
+      </c>
+      <c r="D49" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E49" s="38">
+        <v>0.2145</v>
+      </c>
+      <c r="F49" s="35">
+        <v>19</v>
+      </c>
+      <c r="G49" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H49" s="36">
+        <v>0.11550000000000001</v>
+      </c>
+      <c r="I49" s="37">
+        <v>19</v>
+      </c>
+      <c r="J49" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K49" s="38">
+        <v>0.60819999999999996</v>
+      </c>
+      <c r="L49" s="35">
+        <v>19</v>
+      </c>
+      <c r="M49" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N49" s="36">
+        <v>0.47539999999999999</v>
+      </c>
+      <c r="O49" s="37">
+        <v>19</v>
+      </c>
+      <c r="P49" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q49" s="35">
+        <v>1</v>
+      </c>
+      <c r="R49" s="35">
+        <v>19</v>
+      </c>
+      <c r="S49" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="B50" s="33">
+        <v>0.97909999999999997</v>
+      </c>
+      <c r="C50" s="34">
+        <v>18</v>
+      </c>
+      <c r="D50" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E50" s="38">
+        <v>0.66849999999999998</v>
+      </c>
+      <c r="F50" s="35">
+        <v>18</v>
+      </c>
+      <c r="G50" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H50" s="36">
+        <v>0.16220000000000001</v>
+      </c>
+      <c r="I50" s="37">
+        <v>18</v>
+      </c>
+      <c r="J50" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K50" s="38">
+        <v>3.406E-2</v>
+      </c>
+      <c r="L50" s="35">
+        <v>18</v>
+      </c>
+      <c r="M50" s="40">
+        <v>-4.1549999999999998E-3</v>
+      </c>
+      <c r="N50" s="37">
+        <v>1</v>
+      </c>
+      <c r="O50" s="37">
+        <v>18</v>
+      </c>
+      <c r="P50" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q50" s="38">
+        <v>0.1575</v>
+      </c>
+      <c r="R50" s="35">
+        <v>18</v>
+      </c>
+      <c r="S50" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B51" s="33">
+        <v>1</v>
+      </c>
+      <c r="C51" s="34">
+        <v>29</v>
+      </c>
+      <c r="D51" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E51" s="38">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="F51" s="35">
+        <v>29</v>
+      </c>
+      <c r="G51" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H51" s="36">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="I51" s="37">
+        <v>29</v>
+      </c>
+      <c r="J51" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K51" s="38">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="L51" s="35">
+        <v>29</v>
+      </c>
+      <c r="M51" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N51" s="36">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="O51" s="37">
+        <v>29</v>
+      </c>
+      <c r="P51" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q51" s="38">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="R51" s="35">
+        <v>29</v>
+      </c>
+      <c r="S51" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B52" s="33">
+        <v>1</v>
+      </c>
+      <c r="C52" s="34">
+        <v>30</v>
+      </c>
+      <c r="D52" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E52" s="38">
+        <v>0.53029999999999999</v>
+      </c>
+      <c r="F52" s="35">
+        <v>30</v>
+      </c>
+      <c r="G52" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H52" s="41" t="s">
+        <v>1393</v>
+      </c>
+      <c r="I52" s="37">
+        <v>30</v>
+      </c>
+      <c r="J52" s="36">
+        <v>1.1195E-2</v>
+      </c>
+      <c r="K52" s="38">
+        <v>1.9480000000000001E-2</v>
+      </c>
+      <c r="L52" s="35">
+        <v>30</v>
+      </c>
+      <c r="M52" s="40">
+        <v>3.1099999999999999E-3</v>
+      </c>
+      <c r="N52" s="37">
+        <v>1</v>
+      </c>
+      <c r="O52" s="37">
+        <v>30</v>
+      </c>
+      <c r="P52" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q52" s="38">
+        <v>0.98140000000000005</v>
+      </c>
+      <c r="R52" s="35">
+        <v>30</v>
+      </c>
+      <c r="S52" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B53" s="33">
+        <v>1</v>
+      </c>
+      <c r="C53" s="34">
+        <v>23</v>
+      </c>
+      <c r="D53" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E53" s="38">
+        <v>0.2288</v>
+      </c>
+      <c r="F53" s="35">
+        <v>23</v>
+      </c>
+      <c r="G53" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H53" s="36">
+        <v>4.5450000000000004E-3</v>
+      </c>
+      <c r="I53" s="37">
+        <v>23</v>
+      </c>
+      <c r="J53" s="39">
+        <v>9.0489999999999998E-3</v>
+      </c>
+      <c r="K53" s="38">
+        <v>4.623E-2</v>
+      </c>
+      <c r="L53" s="35">
+        <v>23</v>
+      </c>
+      <c r="M53" s="35">
+        <v>2.8E-3</v>
+      </c>
+      <c r="N53" s="36">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="O53" s="37">
+        <v>23</v>
+      </c>
+      <c r="P53" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q53" s="38">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="R53" s="35">
+        <v>23</v>
+      </c>
+      <c r="S53" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54" s="33">
+        <v>1</v>
+      </c>
+      <c r="C54" s="34">
+        <v>13</v>
+      </c>
+      <c r="D54" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E54" s="38">
+        <v>0.7298</v>
+      </c>
+      <c r="F54" s="35">
+        <v>13</v>
+      </c>
+      <c r="G54" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H54" s="36">
+        <v>0.26050000000000001</v>
+      </c>
+      <c r="I54" s="37">
+        <v>13</v>
+      </c>
+      <c r="J54" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K54" s="38">
+        <v>0.36209999999999998</v>
+      </c>
+      <c r="L54" s="35">
+        <v>13</v>
+      </c>
+      <c r="M54" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N54" s="36">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="O54" s="37">
+        <v>13</v>
+      </c>
+      <c r="P54" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q54" s="35">
+        <v>1</v>
+      </c>
+      <c r="R54" s="35">
+        <v>13</v>
+      </c>
+      <c r="S54" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="s">
+        <v>1394</v>
+      </c>
+      <c r="B55" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C55" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="D55" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="E55" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="F55" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="G55" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="H55" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="I55" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="J55" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="K55" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="L55" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="M55" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="N55" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="O55" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="P55" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="Q55" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="R55" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="S55" s="28" t="s">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
+        <v>656</v>
+      </c>
+      <c r="B56" s="33">
+        <v>0.15740000000000001</v>
+      </c>
+      <c r="C56" s="34">
+        <v>28</v>
+      </c>
+      <c r="D56" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E56" s="42" t="s">
+        <v>1393</v>
+      </c>
+      <c r="F56" s="35">
+        <v>28</v>
+      </c>
+      <c r="G56" s="38">
+        <v>-8.6499999999999994E-2</v>
+      </c>
+      <c r="H56" s="36">
+        <v>6.5009999999999998E-3</v>
+      </c>
+      <c r="I56" s="37">
+        <v>28</v>
+      </c>
+      <c r="J56" s="37">
+        <v>-5.7000000000000002E-2</v>
+      </c>
+      <c r="K56" s="38">
+        <v>0.79549999999999998</v>
+      </c>
+      <c r="L56" s="35">
+        <v>28</v>
+      </c>
+      <c r="M56" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N56" s="36">
+        <v>0.41970000000000002</v>
+      </c>
+      <c r="O56" s="37">
+        <v>28</v>
+      </c>
+      <c r="P56" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q56" s="38">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="R56" s="35">
+        <v>28</v>
+      </c>
+      <c r="S56" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B57" s="33">
+        <v>1</v>
+      </c>
+      <c r="C57" s="34">
+        <v>17</v>
+      </c>
+      <c r="D57" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E57" s="38">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="F57" s="35">
+        <v>17</v>
+      </c>
+      <c r="G57" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H57" s="36">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="I57" s="37">
+        <v>17</v>
+      </c>
+      <c r="J57" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K57" s="35">
+        <v>1</v>
+      </c>
+      <c r="L57" s="35">
+        <v>17</v>
+      </c>
+      <c r="M57" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N57" s="37">
+        <v>1</v>
+      </c>
+      <c r="O57" s="37">
+        <v>17</v>
+      </c>
+      <c r="P57" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q57" s="35">
+        <v>1</v>
+      </c>
+      <c r="R57" s="35">
+        <v>17</v>
+      </c>
+      <c r="S57" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="B58" s="33">
+        <v>1</v>
+      </c>
+      <c r="C58" s="34">
+        <v>16</v>
+      </c>
+      <c r="D58" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E58" s="38">
+        <v>0.37140000000000001</v>
+      </c>
+      <c r="F58" s="35">
+        <v>16</v>
+      </c>
+      <c r="G58" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H58" s="36">
+        <v>0.1575</v>
+      </c>
+      <c r="I58" s="37">
+        <v>16</v>
+      </c>
+      <c r="J58" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K58" s="35">
+        <v>1</v>
+      </c>
+      <c r="L58" s="35">
+        <v>16</v>
+      </c>
+      <c r="M58" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N58" s="37">
+        <v>1</v>
+      </c>
+      <c r="O58" s="37">
+        <v>16</v>
+      </c>
+      <c r="P58" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q58" s="38">
+        <v>0.1575</v>
+      </c>
+      <c r="R58" s="35">
+        <v>16</v>
+      </c>
+      <c r="S58" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
+        <v>1395</v>
+      </c>
+      <c r="B59" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C59" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="D59" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="E59" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="F59" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="G59" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="H59" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="I59" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="J59" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="K59" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="L59" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="M59" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="N59" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="O59" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="P59" s="33" t="s">
+        <v>1385</v>
+      </c>
+      <c r="Q59" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="R59" s="28" t="s">
+        <v>1385</v>
+      </c>
+      <c r="S59" s="28" t="s">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
+        <v>796</v>
+      </c>
+      <c r="B60" s="33">
+        <v>1</v>
+      </c>
+      <c r="C60" s="34">
+        <v>18</v>
+      </c>
+      <c r="D60" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E60" s="38">
+        <v>0.80969999999999998</v>
+      </c>
+      <c r="F60" s="35">
+        <v>18</v>
+      </c>
+      <c r="G60" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H60" s="36">
+        <v>0.9103</v>
+      </c>
+      <c r="I60" s="37">
+        <v>18</v>
+      </c>
+      <c r="J60" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K60" s="35">
+        <v>1</v>
+      </c>
+      <c r="L60" s="35">
+        <v>18</v>
+      </c>
+      <c r="M60" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N60" s="36">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="O60" s="37">
+        <v>18</v>
+      </c>
+      <c r="P60" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q60" s="38">
+        <v>0.93740000000000001</v>
+      </c>
+      <c r="R60" s="35">
+        <v>18</v>
+      </c>
+      <c r="S60" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B61" s="33">
+        <v>1</v>
+      </c>
+      <c r="C61" s="34">
+        <v>22</v>
+      </c>
+      <c r="D61" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E61" s="38">
+        <v>6.404E-2</v>
+      </c>
+      <c r="F61" s="35">
+        <v>22</v>
+      </c>
+      <c r="G61" s="40">
+        <v>-9.4500000000000001E-3</v>
+      </c>
+      <c r="H61" s="36">
+        <v>0.29880000000000001</v>
+      </c>
+      <c r="I61" s="37">
+        <v>22</v>
+      </c>
+      <c r="J61" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K61" s="38">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="L61" s="35">
+        <v>22</v>
+      </c>
+      <c r="M61" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N61" s="36">
+        <v>0.53690000000000004</v>
+      </c>
+      <c r="O61" s="37">
+        <v>22</v>
+      </c>
+      <c r="P61" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q61" s="38">
+        <v>0.15740000000000001</v>
+      </c>
+      <c r="R61" s="35">
+        <v>22</v>
+      </c>
+      <c r="S61" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B62" s="33">
+        <v>1</v>
+      </c>
+      <c r="C62" s="34">
+        <v>26</v>
+      </c>
+      <c r="D62" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E62" s="38">
+        <v>0.33550000000000002</v>
+      </c>
+      <c r="F62" s="35">
+        <v>26</v>
+      </c>
+      <c r="G62" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H62" s="36">
+        <v>0.14360000000000001</v>
+      </c>
+      <c r="I62" s="37">
+        <v>26</v>
+      </c>
+      <c r="J62" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K62" s="38">
+        <v>0.15740000000000001</v>
+      </c>
+      <c r="L62" s="35">
+        <v>26</v>
+      </c>
+      <c r="M62" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N62" s="36">
+        <v>0.97789999999999999</v>
+      </c>
+      <c r="O62" s="37">
+        <v>26</v>
+      </c>
+      <c r="P62" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q62" s="38">
+        <v>2.8869999999999998E-3</v>
+      </c>
+      <c r="R62" s="35">
+        <v>26</v>
+      </c>
+      <c r="S62" s="38">
+        <v>-4.5199999999999997E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B63" s="33">
+        <v>1</v>
+      </c>
+      <c r="C63" s="34">
+        <v>22</v>
+      </c>
+      <c r="D63" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E63" s="38">
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="F63" s="35">
+        <v>22</v>
+      </c>
+      <c r="G63" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H63" s="36">
+        <v>0.81320000000000003</v>
+      </c>
+      <c r="I63" s="37">
+        <v>22</v>
+      </c>
+      <c r="J63" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K63" s="38">
+        <v>0.56189999999999996</v>
+      </c>
+      <c r="L63" s="35">
+        <v>22</v>
+      </c>
+      <c r="M63" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N63" s="36">
+        <v>0.15740000000000001</v>
+      </c>
+      <c r="O63" s="37">
+        <v>22</v>
+      </c>
+      <c r="P63" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q63" s="35">
+        <v>1</v>
+      </c>
+      <c r="R63" s="35">
+        <v>22</v>
+      </c>
+      <c r="S63" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
+        <v>859</v>
+      </c>
+      <c r="B64" s="33">
+        <v>1</v>
+      </c>
+      <c r="C64" s="34">
+        <v>26</v>
+      </c>
+      <c r="D64" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E64" s="38">
+        <v>2.6489999999999999E-3</v>
+      </c>
+      <c r="F64" s="35">
+        <v>26</v>
+      </c>
+      <c r="G64" s="35">
+        <v>-8.5000000000000006E-3</v>
+      </c>
+      <c r="H64" s="36">
+        <v>1.52E-2</v>
+      </c>
+      <c r="I64" s="37">
+        <v>26</v>
+      </c>
+      <c r="J64" s="36">
+        <v>-1.55E-2</v>
+      </c>
+      <c r="K64" s="38">
+        <v>0.84719999999999995</v>
+      </c>
+      <c r="L64" s="35">
+        <v>26</v>
+      </c>
+      <c r="M64" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N64" s="36">
+        <v>0.1148</v>
+      </c>
+      <c r="O64" s="37">
+        <v>26</v>
+      </c>
+      <c r="P64" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q64" s="38">
+        <v>2.5590000000000002E-2</v>
+      </c>
+      <c r="R64" s="35">
+        <v>26</v>
+      </c>
+      <c r="S64" s="40">
+        <v>4.3099999999999996E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
+        <v>867</v>
+      </c>
+      <c r="B65" s="33">
+        <v>1</v>
+      </c>
+      <c r="C65" s="34">
+        <v>27</v>
+      </c>
+      <c r="D65" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E65" s="38">
+        <v>2.6259999999999999E-3</v>
+      </c>
+      <c r="F65" s="35">
+        <v>26</v>
+      </c>
+      <c r="G65" s="40">
+        <v>3.2100000000000002E-3</v>
+      </c>
+      <c r="H65" s="41" t="s">
+        <v>1393</v>
+      </c>
+      <c r="I65" s="37">
+        <v>27</v>
+      </c>
+      <c r="J65" s="39">
+        <v>7.6490000000000004E-3</v>
+      </c>
+      <c r="K65" s="35">
+        <v>1</v>
+      </c>
+      <c r="L65" s="35">
+        <v>27</v>
+      </c>
+      <c r="M65" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N65" s="37">
+        <v>1</v>
+      </c>
+      <c r="O65" s="37">
+        <v>27</v>
+      </c>
+      <c r="P65" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q65" s="35">
+        <v>1</v>
+      </c>
+      <c r="R65" s="35">
+        <v>27</v>
+      </c>
+      <c r="S65" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
+        <v>578</v>
+      </c>
+      <c r="B66" s="33">
+        <v>1</v>
+      </c>
+      <c r="C66" s="34">
+        <v>19</v>
+      </c>
+      <c r="D66" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E66" s="38">
+        <v>0.30230000000000001</v>
+      </c>
+      <c r="F66" s="35">
+        <v>19</v>
+      </c>
+      <c r="G66" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H66" s="36">
+        <v>0.60819999999999996</v>
+      </c>
+      <c r="I66" s="37">
+        <v>19</v>
+      </c>
+      <c r="J66" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K66" s="38">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="L66" s="35">
+        <v>19</v>
+      </c>
+      <c r="M66" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N66" s="36">
+        <v>0.30470000000000003</v>
+      </c>
+      <c r="O66" s="37">
+        <v>19</v>
+      </c>
+      <c r="P66" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q66" s="38">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="R66" s="35">
+        <v>19</v>
+      </c>
+      <c r="S66" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
+        <v>990</v>
+      </c>
+      <c r="B67" s="33">
+        <v>1</v>
+      </c>
+      <c r="C67" s="34">
+        <v>24</v>
+      </c>
+      <c r="D67" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E67" s="38">
+        <v>0.13150000000000001</v>
+      </c>
+      <c r="F67" s="35">
+        <v>24</v>
+      </c>
+      <c r="G67" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H67" s="36">
+        <v>0.1071</v>
+      </c>
+      <c r="I67" s="37">
+        <v>24</v>
+      </c>
+      <c r="J67" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K67" s="38">
+        <v>0.30730000000000002</v>
+      </c>
+      <c r="L67" s="35">
+        <v>24</v>
+      </c>
+      <c r="M67" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N67" s="36">
+        <v>0.59830000000000005</v>
+      </c>
+      <c r="O67" s="37">
+        <v>24</v>
+      </c>
+      <c r="P67" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q67" s="38">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="R67" s="35">
+        <v>24</v>
+      </c>
+      <c r="S67" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
+        <v>969</v>
+      </c>
+      <c r="B68" s="33">
+        <v>1</v>
+      </c>
+      <c r="C68" s="34">
+        <v>26</v>
+      </c>
+      <c r="D68" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E68" s="38">
+        <v>0.17</v>
+      </c>
+      <c r="F68" s="35">
+        <v>26</v>
+      </c>
+      <c r="G68" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H68" s="36">
+        <v>5.67E-2</v>
+      </c>
+      <c r="I68" s="37">
+        <v>26</v>
+      </c>
+      <c r="J68" s="36">
+        <v>-4.1450000000000001E-2</v>
+      </c>
+      <c r="K68" s="38">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="L68" s="35">
+        <v>26</v>
+      </c>
+      <c r="M68" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N68" s="36">
+        <v>0.15740000000000001</v>
+      </c>
+      <c r="O68" s="37">
+        <v>26</v>
+      </c>
+      <c r="P68" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q68" s="38">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="R68" s="35">
+        <v>26</v>
+      </c>
+      <c r="S68" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
+        <v>966</v>
+      </c>
+      <c r="B69" s="33">
+        <v>1</v>
+      </c>
+      <c r="C69" s="34">
+        <v>25</v>
+      </c>
+      <c r="D69" s="33" t="s">
+        <v>1383</v>
+      </c>
+      <c r="E69" s="38">
+        <v>0.20710000000000001</v>
+      </c>
+      <c r="F69" s="35">
+        <v>25</v>
+      </c>
+      <c r="G69" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H69" s="36">
+        <v>0.43659999999999999</v>
+      </c>
+      <c r="I69" s="37">
+        <v>25</v>
+      </c>
+      <c r="J69" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K69" s="38">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="L69" s="35">
+        <v>25</v>
+      </c>
+      <c r="M69" s="35" t="s">
+        <v>1383</v>
+      </c>
+      <c r="N69" s="36">
+        <v>0.15740000000000001</v>
+      </c>
+      <c r="O69" s="37">
+        <v>25</v>
+      </c>
+      <c r="P69" s="37" t="s">
+        <v>1383</v>
+      </c>
+      <c r="Q69" s="38">
+        <v>0.31730000000000003</v>
+      </c>
+      <c r="R69" s="35">
+        <v>25</v>
+      </c>
+      <c r="S69" s="35" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="Q1:S1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2697"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="N1" sqref="A1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5644,9 +9905,11 @@
     <col min="1" max="1" width="11.85546875" style="6" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" style="5" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="9" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="16" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.28515625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="3" customWidth="1"/>
+    <col min="11" max="13" width="11.28515625" style="3" customWidth="1"/>
+    <col min="14" max="16" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>

</xml_diff>